<commit_message>
added source tablets, update plans
</commit_message>
<xml_diff>
--- a/Scripts/python/SourceTables/Talismans.xlsx
+++ b/Scripts/python/SourceTables/Talismans.xlsx
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +997,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="99" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>76</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>79</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>82</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>85</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>88</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>91</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>94</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>

</xml_diff>